<commit_message>
first attempt tbable 6th matrch
</commit_message>
<xml_diff>
--- a/stats/austroplaca/month_PAR_stats_X3.xlsx
+++ b/stats/austroplaca/month_PAR_stats_X3.xlsx
@@ -570,13 +570,13 @@
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>103.646153846154</v>
+        <v>54.7752976190476</v>
       </c>
       <c r="D13" t="n">
-        <v>404</v>
+        <v>662</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>91.9761549925485</v>
+        <v>91.8392857142857</v>
       </c>
       <c r="D17" t="n">
         <v>575</v>

</xml_diff>